<commit_message>
Test cases for lab07 - Ethan
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zee/development/CS151_labs/Lab7/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eadch\PycharmProjects\cs151-lab7-ethan_liv_lab7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF27D802-FB15-694F-BF0B-8F3CB3EC9386}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFEA0719-904E-4130-B496-5A9814DCD113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{078FF010-DC04-EB46-847F-52BBCCEEE85C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="6" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
   <si>
     <t>&lt;-- final overall cost</t>
   </si>
@@ -58,12 +58,24 @@
   </si>
   <si>
     <t>cost/sqft</t>
+  </si>
+  <si>
+    <t>hardwood</t>
+  </si>
+  <si>
+    <t>carpet</t>
+  </si>
+  <si>
+    <t>tile</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -205,18 +217,32 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="3" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="40% - Accent5" xfId="2" builtinId="47"/>
@@ -273,9 +299,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -313,7 +339,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -419,7 +445,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -561,7 +587,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -572,10 +598,10 @@
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" bestFit="1" customWidth="1"/>
@@ -585,23 +611,23 @@
     <col min="7" max="7" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="G1" s="7" t="s">
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="G1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+    <row r="2" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -610,57 +636,117 @@
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="11" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
+      <c r="G2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="6">
+        <v>1.39</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="8">
+        <v>14</v>
+      </c>
+      <c r="C3" s="8">
+        <v>15</v>
+      </c>
+      <c r="D3" s="12">
+        <f>(B3*C3)*H2</f>
+        <v>291.89999999999998</v>
+      </c>
       <c r="E3" s="1"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
+      <c r="G3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="6">
+        <v>3.99</v>
+      </c>
     </row>
-    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
+    <row r="4" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="8">
+        <v>10</v>
+      </c>
+      <c r="C4" s="8">
+        <v>15</v>
+      </c>
+      <c r="D4" s="12">
+        <f>(B4*C4)*H3</f>
+        <v>598.5</v>
+      </c>
       <c r="E4" s="1"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
+      <c r="G4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="6">
+        <v>4.99</v>
+      </c>
     </row>
-    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
+    <row r="5" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="8">
+        <v>12</v>
+      </c>
+      <c r="C5" s="8">
+        <v>16</v>
+      </c>
+      <c r="D5" s="12">
+        <f>(B5*C5)*H4</f>
+        <v>958.08</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
+    <row r="6" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A6" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="8">
+        <v>9</v>
+      </c>
+      <c r="C6" s="8">
+        <v>11</v>
+      </c>
+      <c r="D6" s="12">
+        <f>(B6*C6)*H4</f>
+        <v>494.01000000000005</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3"/>
+    <row r="7" spans="1:8" ht="21" x14ac:dyDescent="0.5">
+      <c r="A7" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8">
+        <v>13</v>
+      </c>
+      <c r="C7" s="8">
+        <v>10</v>
+      </c>
+      <c r="D7" s="12">
+        <f>(B7*C7)*H2</f>
+        <v>180.7</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
+      <c r="D8" s="12">
+        <f>SUM(D3:D7)</f>
+        <v>2523.19</v>
+      </c>
       <c r="E8" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>